<commit_message>
Add replanting: Loop which calculates for each year: - tree diebacks because auf risks, dependent on the tree ages - resulting max. yield depending on ages - resulting tree quantity and quality
</commit_message>
<xml_diff>
--- a/Data/data_estimates.xlsx
+++ b/Data/data_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2E1B63-510F-4D4A-8BE2-F877BBAAFC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AAF02A-41C8-454F-AC06-3867223603BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="-8460" windowWidth="14610" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="28680" yWindow="1020" windowWidth="29040" windowHeight="15720" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="78">
   <si>
     <t>variable</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>tree_establishment_costs</t>
+  </si>
+  <si>
+    <t>fruit_labor_replanting_mean_h</t>
+  </si>
+  <si>
+    <t>fruit_labor_replanting_var</t>
   </si>
 </sst>
 </file>
@@ -360,16 +366,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -707,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +915,7 @@
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C10">
@@ -921,10 +924,10 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="4">
         <v>30</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G10" t="s">
@@ -935,7 +938,7 @@
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C11">
@@ -947,10 +950,10 @@
       <c r="E11">
         <v>0.5</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -958,7 +961,7 @@
       <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C12">
@@ -970,10 +973,10 @@
       <c r="E12">
         <v>9</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -981,7 +984,7 @@
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C13">
@@ -993,10 +996,10 @@
       <c r="E13">
         <v>8</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1073,7 +1076,7 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C17">
@@ -1082,10 +1085,10 @@
       <c r="D17" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="4">
         <v>0.9</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1151,7 +1154,7 @@
       <c r="F20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1219,7 +1222,7 @@
       <c r="A24" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C24">
@@ -1228,10 +1231,10 @@
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="4">
         <v>30</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1239,7 +1242,7 @@
       <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C25">
@@ -1251,7 +1254,7 @@
       <c r="E25">
         <v>0.2</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1259,7 +1262,7 @@
       <c r="A26" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C26">
@@ -1271,10 +1274,10 @@
       <c r="E26">
         <v>6</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1282,7 +1285,7 @@
       <c r="A27" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C27">
@@ -1294,10 +1297,10 @@
       <c r="E27">
         <v>45</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1305,7 +1308,7 @@
       <c r="A28" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C28">
@@ -1317,7 +1320,7 @@
       <c r="E28">
         <v>0.15</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1325,7 +1328,7 @@
       <c r="A29" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C29">
@@ -1337,7 +1340,7 @@
       <c r="E29">
         <v>0.9</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1422,7 +1425,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1442,13 +1445,13 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="6">
         <f>(10/60)</f>
         <v>0.16666666666666666</v>
       </c>
@@ -1463,10 +1466,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C36">
@@ -1475,13 +1478,13 @@
       <c r="D36" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="4">
         <v>40000</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1489,7 +1492,7 @@
       <c r="A37" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C37">
@@ -1498,10 +1501,10 @@
       <c r="D37" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="4">
         <v>0.2</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1509,7 +1512,7 @@
       <c r="A38" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C38">
@@ -1518,10 +1521,10 @@
       <c r="D38" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="4">
         <v>10</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1529,7 +1532,7 @@
       <c r="A39" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C39">
@@ -1538,10 +1541,10 @@
       <c r="D39" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="4">
         <v>10</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1549,7 +1552,7 @@
       <c r="A40" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C40">
@@ -1558,10 +1561,10 @@
       <c r="D40" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="4">
         <v>0.7</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1586,15 +1589,41 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="5"/>
+      <c r="A42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <v>0.3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
-      <c r="E43" s="4"/>
+      <c r="A43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>0.2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.7</v>
+      </c>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adding subsidies: - GLOETZ (Grundstütze, flächenbezogen, 1. Säule GAP) - HALM2 E2.1 (Beibehaltung FS, Säule 2) - HALM2 E 2.2 (Neupflanzungen)
Next ToDo:
- refines risks impacts!
- maint+est costs in detail
</commit_message>
<xml_diff>
--- a/Data/data_estimates.xlsx
+++ b/Data/data_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AAF02A-41C8-454F-AC06-3867223603BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F1509F-39AE-4672-B97E-8967C51BECE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1020" windowWidth="29040" windowHeight="15720" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="47895" yWindow="1140" windowWidth="9810" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="90">
   <si>
     <t>variable</t>
   </si>
@@ -122,9 +122,6 @@
     <t>supply_chain_invest_mean_h</t>
   </si>
   <si>
-    <t>supply_chain_invest_var_h</t>
-  </si>
-  <si>
     <t>Hours spent annually to keep trading contacts</t>
   </si>
   <si>
@@ -134,18 +131,12 @@
     <t>Eur per kg</t>
   </si>
   <si>
-    <t>Price for walnut direct marketing</t>
-  </si>
-  <si>
     <t>walnut_price_direct_Eur_per_kg</t>
   </si>
   <si>
     <t>walnut_price_wholesale_Eur_per_kg</t>
   </si>
   <si>
-    <t>Price for walnut wholesale market</t>
-  </si>
-  <si>
     <t>risk_yearly_drought</t>
   </si>
   <si>
@@ -218,12 +209,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>first yield after planting</t>
-  </si>
-  <si>
-    <t>HeH left out?!</t>
-  </si>
-  <si>
     <t>percent</t>
   </si>
   <si>
@@ -270,6 +255,57 @@
   </si>
   <si>
     <t>fruit_labor_replanting_var</t>
+  </si>
+  <si>
+    <t>supply_chain_invest_var</t>
+  </si>
+  <si>
+    <t>tree_subsidies_GLOETZ_annual_Eur_per_ha</t>
+  </si>
+  <si>
+    <t>Eur/ha</t>
+  </si>
+  <si>
+    <t>Einkommensstütze (GAP-Direktzahleung 1. Säule)</t>
+  </si>
+  <si>
+    <t>Eur/tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eur/tree </t>
+  </si>
+  <si>
+    <t>HALM 2.1 (Pflege von Agroforst, . Säule ökoregelung)</t>
+  </si>
+  <si>
+    <t>HALM 2.2 (Neupflanzung/Baum, Pflanzjahr)</t>
+  </si>
+  <si>
+    <t>HALM 2.2 (Neupflanzung/Baum, Folgejahre bis 5. Jahr)</t>
+  </si>
+  <si>
+    <t>Price for walnut direct marketing (Verkaufspreis, bio)</t>
+  </si>
+  <si>
+    <t>Price for walnut wholesale market (Erzeugerpreis, bio)</t>
+  </si>
+  <si>
+    <t>first yield after planting (8)</t>
+  </si>
+  <si>
+    <t>Vollertrag (15.-50. Jahr)</t>
+  </si>
+  <si>
+    <t>15-60 --&gt; we take optimum</t>
+  </si>
+  <si>
+    <t>tree_subsidies_HALM_2_1_annual_Eur_per_tree</t>
+  </si>
+  <si>
+    <t>tree_subsidies_HALM_2_2_y1_Eur_per_tree</t>
+  </si>
+  <si>
+    <t>tree_subsidies_HALM_2_2_y2_5_Eur_per_tree</t>
   </si>
 </sst>
 </file>
@@ -366,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -374,6 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -710,13 +747,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -931,12 +968,12 @@
         <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>7</v>
@@ -954,35 +991,35 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>9</v>
@@ -994,18 +1031,18 @@
         <v>8</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>7</v>
@@ -1023,12 +1060,12 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>7</v>
@@ -1046,12 +1083,12 @@
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>7</v>
@@ -1069,12 +1106,12 @@
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>7</v>
@@ -1094,7 +1131,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>7</v>
@@ -1112,12 +1149,12 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>7</v>
@@ -1137,7 +1174,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>7</v>
@@ -1155,12 +1192,12 @@
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>7</v>
@@ -1180,7 +1217,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>7</v>
@@ -1200,7 +1237,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>7</v>
@@ -1220,27 +1257,30 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="4">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>7</v>
@@ -1255,58 +1295,58 @@
         <v>0.2</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G26" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C27">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>7</v>
@@ -1321,12 +1361,12 @@
         <v>0.15</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>7</v>
@@ -1341,12 +1381,12 @@
         <v>0.9</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>9</v>
@@ -1366,7 +1406,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>7</v>
@@ -1386,7 +1426,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>9</v>
@@ -1406,7 +1446,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>7</v>
@@ -1426,7 +1466,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>9</v>
@@ -1446,7 +1486,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>7</v>
@@ -1467,7 +1507,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>9</v>
@@ -1485,12 +1525,12 @@
         <v>17</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>7</v>
@@ -1510,7 +1550,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>9</v>
@@ -1530,7 +1570,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>9</v>
@@ -1550,7 +1590,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>9</v>
@@ -1570,7 +1610,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>9</v>
@@ -1590,7 +1630,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>9</v>
@@ -1610,7 +1650,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>7</v>
@@ -1627,28 +1667,87 @@
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="5"/>
+      <c r="A44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44">
+        <v>157</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="4">
+        <v>157</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="5"/>
+      <c r="A45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45">
+        <v>9</v>
+      </c>
+      <c r="E45" s="4">
+        <v>9</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="5"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="5"/>
+      <c r="A46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46">
+        <v>90</v>
+      </c>
+      <c r="E46" s="4">
+        <v>90</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G46" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="5"/>
+      <c r="A47" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="E47" s="4">
+        <v>9</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G47" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>

</xml_diff>

<commit_message>
Correction of: - subsidies (5-year payments) - risks (different influences on dieback, quanti and quali)
</commit_message>
<xml_diff>
--- a/Data/data_estimates.xlsx
+++ b/Data/data_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F1509F-39AE-4672-B97E-8967C51BECE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A544D56-DC2F-4A38-A7D0-ACA24D7F50E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="1140" windowWidth="9810" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="47895" yWindow="0" windowWidth="9810" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="103">
   <si>
     <t>variable</t>
   </si>
@@ -260,9 +260,6 @@
     <t>supply_chain_invest_var</t>
   </si>
   <si>
-    <t>tree_subsidies_GLOETZ_annual_Eur_per_ha</t>
-  </si>
-  <si>
     <t>Eur/ha</t>
   </si>
   <si>
@@ -306,13 +303,55 @@
   </si>
   <si>
     <t>tree_subsidies_HALM_2_2_y2_5_Eur_per_tree</t>
+  </si>
+  <si>
+    <t>tree_subsidies_GLOEZ_annual_Eur_per_ha</t>
+  </si>
+  <si>
+    <t>risk_disease_dieback_mean</t>
+  </si>
+  <si>
+    <t>absolute</t>
+  </si>
+  <si>
+    <t>risk_disease_dieback_var</t>
+  </si>
+  <si>
+    <t>risk_drought_dieback_mean</t>
+  </si>
+  <si>
+    <t>risk_drought_dieback_var</t>
+  </si>
+  <si>
+    <t>risk_disease_yield_red_mean</t>
+  </si>
+  <si>
+    <t>risk_disease_yield_red_var</t>
+  </si>
+  <si>
+    <t>risk_frost_yield_red_mean</t>
+  </si>
+  <si>
+    <t>risk_frost_yield_red_var</t>
+  </si>
+  <si>
+    <t>risk_disease_quali_red_mean</t>
+  </si>
+  <si>
+    <t>risk_disease_quali_red_var</t>
+  </si>
+  <si>
+    <t>risk_frost_quali_red_mean</t>
+  </si>
+  <si>
+    <t>risk_frost_quali_red_var</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +363,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -402,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -411,6 +456,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -745,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,7 +1061,7 @@
         <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1037,7 +1084,7 @@
         <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1269,13 +1316,13 @@
         <v>8</v>
       </c>
       <c r="E24" s="4">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>54</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1318,7 +1365,7 @@
         <v>56</v>
       </c>
       <c r="G26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1341,7 +1388,7 @@
         <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1668,7 +1715,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>22</v>
@@ -1683,15 +1730,15 @@
         <v>157</v>
       </c>
       <c r="F44" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>22</v>
@@ -1703,15 +1750,15 @@
         <v>9</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>22</v>
@@ -1723,15 +1770,15 @@
         <v>90</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>22</v>
@@ -1743,19 +1790,252 @@
         <v>9</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
-      <c r="B48" s="5"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="5"/>
+      <c r="A48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>0.1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>0.1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>0.1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>0.1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>0.1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>0.1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>0.1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>0.1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>0.05</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>0.1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <v>0.05</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59">
+        <v>0.1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated: - risk influence - took out supply chain
=> take this version for interim presentation
</commit_message>
<xml_diff>
--- a/Data/data_estimates.xlsx
+++ b/Data/data_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A544D56-DC2F-4A38-A7D0-ACA24D7F50E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188613BB-6038-44F8-8782-CF798669488C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="0" windowWidth="9810" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="28680" yWindow="-8580" windowWidth="29040" windowHeight="15720" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -455,9 +455,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -794,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1321,7 +1318,7 @@
       <c r="F24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1519,13 +1516,13 @@
         <v>9</v>
       </c>
       <c r="C34">
+        <v>0.25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="4">
         <v>0.5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="4">
-        <v>1</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>18</v>
@@ -1603,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="4">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>18</v>
@@ -1629,7 +1626,7 @@
         <v>8</v>
       </c>
       <c r="E39" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>18</v>
@@ -1669,7 +1666,7 @@
         <v>8</v>
       </c>
       <c r="E41" s="4">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>17</v>
@@ -1732,7 +1729,7 @@
       <c r="F44" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1835,7 +1832,7 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -1847,10 +1844,10 @@
       <c r="D50" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E50" s="4">
         <v>0.15</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="5" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1867,10 +1864,10 @@
       <c r="D51" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E51" s="4">
         <v>0.2</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="5" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1910,12 +1907,12 @@
       <c r="E53" s="4">
         <v>0.9</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="F53" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -1927,15 +1924,15 @@
       <c r="D54" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="4">
         <v>0.3</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F54" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -1947,7 +1944,7 @@
       <c r="D55" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E55" s="4">
         <v>0.5</v>
       </c>
       <c r="F55" s="5" t="s">
@@ -1990,12 +1987,12 @@
       <c r="E57" s="4">
         <v>0.2</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -2007,15 +2004,15 @@
       <c r="D58" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="8">
+      <c r="E58" s="4">
         <v>0.2</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -2027,7 +2024,7 @@
       <c r="D59" t="s">
         <v>8</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E59" s="4">
         <v>0.2</v>
       </c>
       <c r="F59" s="5" t="s">

</xml_diff>

<commit_message>
Code reviewed: - logic check - comments for explanations
BUT not simplified, rather:
- added supply chain
- added investition subsidy scenario
</commit_message>
<xml_diff>
--- a/Data/data_estimates.xlsx
+++ b/Data/data_estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188613BB-6038-44F8-8782-CF798669488C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2889837A-77CC-4CEF-A8A6-7265034246D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-8580" windowWidth="29040" windowHeight="15720" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
@@ -791,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1563,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="E36" s="4">
-        <v>40000</v>
+        <v>25000</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Added state variable plots: - Fruit yield quantity, revenue - dieback numbers - labor hours
ToDo. get cclear about planting labor hours - sparated for replanbtings and establishment?
- Next step. include data from agency; hay refinement
</commit_message>
<xml_diff>
--- a/Data/data_estimates.xlsx
+++ b/Data/data_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7A3FC7-208D-4207-8E24-637AF0363776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D232817E-175A-4034-A987-CD107B9B6EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8580" windowWidth="29040" windowHeight="15720" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="106">
   <si>
     <t>variable</t>
   </si>
@@ -345,6 +345,15 @@
   </si>
   <si>
     <t>risk_frost_quali_red_var</t>
+  </si>
+  <si>
+    <t>tree_labor_establishment_var_h_per_tree</t>
+  </si>
+  <si>
+    <t>tree_labor_planting_mean_h_per_tree</t>
+  </si>
+  <si>
+    <t>Heh. Bestellung etc neuer Bääume?! Oder weg</t>
   </si>
 </sst>
 </file>
@@ -447,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -455,6 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -789,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,41 +1662,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>70</v>
+    <row r="41" spans="1:7" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>104</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C41">
-        <v>5000</v>
+        <v>0.5</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="4">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>71</v>
+      <c r="A42" t="s">
+        <v>103</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="4">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>18</v>
@@ -1694,94 +1704,91 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C43">
-        <v>0.2</v>
+        <v>5000</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>10000</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>157</v>
+        <v>0.3</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="4">
-        <v>157</v>
+        <v>0.75</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G44" t="s">
-        <v>75</v>
+        <v>18</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>9</v>
+        <v>0.2</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="4">
-        <v>9</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G45" t="s">
-        <v>78</v>
-      </c>
+        <v>0.7</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C46">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="D46" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="4">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>22</v>
@@ -1799,70 +1806,78 @@
         <v>76</v>
       </c>
       <c r="G47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48">
         <v>90</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48">
-        <v>0.1</v>
-      </c>
       <c r="D48" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="4">
+        <v>90</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="4">
+        <v>9</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>0.1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="4">
         <v>0.6</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49">
-        <v>0.1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50">
-        <v>0.1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="4">
-        <v>0.15</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>94</v>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>7</v>
@@ -1874,15 +1889,13 @@
         <v>8</v>
       </c>
       <c r="E51" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.9</v>
+      </c>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>7</v>
@@ -1894,15 +1907,15 @@
         <v>8</v>
       </c>
       <c r="E52" s="4">
-        <v>0.9</v>
+        <v>0.15</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>96</v>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>94</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>7</v>
@@ -1914,15 +1927,15 @@
         <v>8</v>
       </c>
       <c r="E53" s="4">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>7</v>
@@ -1934,15 +1947,15 @@
         <v>8</v>
       </c>
       <c r="E54" s="4">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>7</v>
@@ -1954,35 +1967,35 @@
         <v>8</v>
       </c>
       <c r="E55" s="4">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C56">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="4">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>7</v>
@@ -1994,15 +2007,15 @@
         <v>8</v>
       </c>
       <c r="E57" s="4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>7</v>
@@ -2014,15 +2027,15 @@
         <v>8</v>
       </c>
       <c r="E58" s="4">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>7</v>
@@ -2037,6 +2050,46 @@
         <v>0.2</v>
       </c>
       <c r="F59" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>0.05</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61">
+        <v>0.1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Include agency data: - establishment costs - fetilizer, certificates (included as data_agency for clearance)
ToDo:
tree-age-specific
-> pruning, mainteance
-> yield values
</commit_message>
<xml_diff>
--- a/Data/data_estimates.xlsx
+++ b/Data/data_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D232817E-175A-4034-A987-CD107B9B6EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388E00D5-42A8-4611-BF1A-CE227AC612CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="93">
   <si>
     <t>variable</t>
   </si>
@@ -101,15 +101,9 @@
     <t>Variance of labor hours for hay harvest</t>
   </si>
   <si>
-    <t>labor_wage_Eur_per_h_brutto</t>
-  </si>
-  <si>
     <t>const</t>
   </si>
   <si>
-    <t>Brutto cost for labor work per hour</t>
-  </si>
-  <si>
     <t>hay_costs_establishment_Eur</t>
   </si>
   <si>
@@ -128,15 +122,6 @@
     <t>Variance in hours spent to keep trading contacts</t>
   </si>
   <si>
-    <t>Eur per kg</t>
-  </si>
-  <si>
-    <t>walnut_price_direct_Eur_per_kg</t>
-  </si>
-  <si>
-    <t>walnut_price_wholesale_Eur_per_kg</t>
-  </si>
-  <si>
     <t>risk_yearly_drought</t>
   </si>
   <si>
@@ -230,15 +215,6 @@
     <t>timber_labor_harvest_var_h</t>
   </si>
   <si>
-    <t>Harvest machinery</t>
-  </si>
-  <si>
-    <t>fruit_price_machinery_mean_Eur</t>
-  </si>
-  <si>
-    <t>fruit_price_machinery_var_Eur</t>
-  </si>
-  <si>
     <t>fruit_labor_harvest_h_per_kg</t>
   </si>
   <si>
@@ -251,12 +227,6 @@
     <t>tree_establishment_costs</t>
   </si>
   <si>
-    <t>fruit_labor_replanting_mean_h</t>
-  </si>
-  <si>
-    <t>fruit_labor_replanting_var</t>
-  </si>
-  <si>
     <t>supply_chain_invest_var</t>
   </si>
   <si>
@@ -281,12 +251,6 @@
     <t>HALM 2.2 (Neupflanzung/Baum, Folgejahre bis 5. Jahr)</t>
   </si>
   <si>
-    <t>Price for walnut direct marketing (Verkaufspreis, bio)</t>
-  </si>
-  <si>
-    <t>Price for walnut wholesale market (Erzeugerpreis, bio)</t>
-  </si>
-  <si>
     <t>first yield after planting (8)</t>
   </si>
   <si>
@@ -351,9 +315,6 @@
   </si>
   <si>
     <t>tree_labor_planting_mean_h_per_tree</t>
-  </si>
-  <si>
-    <t>Heh. Bestellung etc neuer Bääume?! Oder weg</t>
   </si>
 </sst>
 </file>
@@ -456,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -464,7 +425,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -799,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,7 +875,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
@@ -935,7 +895,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
@@ -958,7 +918,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
@@ -980,164 +940,161 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
+      <c r="A9" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>0.15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4">
-        <v>30</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C11">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11">
-        <v>0.5</v>
+      <c r="E11" s="4">
+        <v>0.8</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>0.2</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E12">
-        <v>12</v>
+      <c r="E12" s="4">
+        <v>0.7</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>0.05</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="E13">
-        <v>5</v>
+      <c r="E13" s="4">
+        <v>0.15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C15">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="4">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1148,24 +1105,21 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="4">
-        <v>0.15</v>
+        <v>0.9</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G16" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>7</v>
@@ -1182,10 +1136,13 @@
       <c r="F17" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>7</v>
@@ -1202,13 +1159,10 @@
       <c r="F18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G18" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>7</v>
@@ -1228,7 +1182,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>7</v>
@@ -1244,9 +1198,6 @@
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="G20" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1254,24 +1205,27 @@
         <v>43</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>0.1</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="4">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>13</v>
+        <v>49</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>7</v>
@@ -1282,59 +1236,62 @@
       <c r="D22" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="4">
-        <v>0.9</v>
+      <c r="E22">
+        <v>0.2</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>0.1</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="4">
-        <v>0.9</v>
+      <c r="E23">
+        <v>9</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>13</v>
+        <v>51</v>
+      </c>
+      <c r="G23" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C24">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="4">
-        <v>90</v>
+      <c r="E24">
+        <v>21</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G24" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>7</v>
@@ -1346,61 +1303,55 @@
         <v>8</v>
       </c>
       <c r="E25">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C26">
-        <v>7</v>
+        <v>0.8</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26">
-        <v>9</v>
+        <v>0.9</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>51</v>
+      <c r="A27" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C27">
-        <v>14</v>
+        <v>0.5</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
-      <c r="E27">
-        <v>21</v>
+      <c r="E27" s="4">
+        <v>1.5</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>52</v>
+      <c r="A28" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>7</v>
@@ -1411,492 +1362,488 @@
       <c r="D28" t="s">
         <v>8</v>
       </c>
-      <c r="E28">
-        <v>0.15</v>
+      <c r="E28" s="4">
+        <v>0.2</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>53</v>
+      <c r="A29" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>0.8</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
-      <c r="E29">
-        <v>0.9</v>
+      <c r="E29" s="4">
+        <v>40</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C30">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="4">
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C31">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="6">
+        <f>(10/60)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>0.25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>60</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32">
-        <v>20</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="4">
-        <v>40</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33">
-        <v>0.2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C34">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>63</v>
+      <c r="A35" t="s">
+        <v>61</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="6">
-        <f>(10/60)</f>
-        <v>0.16666666666666666</v>
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>0.2</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="4">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C36">
-        <v>20000</v>
+        <v>0.5</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="4">
-        <v>25000</v>
+        <v>1</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C37">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="4">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>67</v>
+      <c r="A38" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C38">
-        <v>0.25</v>
+        <v>5000</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="4">
-        <v>0.5</v>
+        <v>10000</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39">
+        <v>157</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="4">
+        <v>157</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="4">
+        <v>9</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G40" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="5" t="s">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41">
+        <v>90</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="4">
+        <v>90</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42">
         <v>9</v>
       </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="4">
-        <v>5</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="4">
         <v>9</v>
       </c>
-      <c r="C40">
-        <v>0.2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>104</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41">
-        <v>0.5</v>
-      </c>
-      <c r="D41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="4">
-        <v>1</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42">
-        <v>0.5</v>
-      </c>
-      <c r="D42" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="4">
-        <v>0.8</v>
-      </c>
       <c r="F42" s="5" t="s">
-        <v>18</v>
+        <v>66</v>
+      </c>
+      <c r="G42" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>5000</v>
+        <v>0.1</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="4">
-        <v>10000</v>
+        <v>0.6</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>105</v>
-      </c>
+        <v>0.9</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C45">
+        <v>0.1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>0.1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="4">
         <v>0.2</v>
       </c>
-      <c r="D45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46">
-        <v>157</v>
-      </c>
-      <c r="D46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="4">
-        <v>157</v>
-      </c>
       <c r="F46" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G46" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>9</v>
+        <v>0.1</v>
       </c>
       <c r="D47" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="4">
-        <v>9</v>
+        <v>0.9</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>0.1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>0.1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>0.1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48">
-        <v>90</v>
-      </c>
-      <c r="D48" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="4">
-        <v>90</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G48" t="s">
+      <c r="B51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>0.05</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49">
-        <v>9</v>
-      </c>
-      <c r="D49" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="4">
-        <v>9</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50">
-        <v>0.1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51">
-        <v>0.1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="B52" s="5" t="s">
         <v>7</v>
       </c>
@@ -1907,21 +1854,21 @@
         <v>8</v>
       </c>
       <c r="E52" s="4">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>94</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C53">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D53" t="s">
         <v>8</v>
@@ -1930,12 +1877,12 @@
         <v>0.2</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>7</v>
@@ -1947,150 +1894,10 @@
         <v>8</v>
       </c>
       <c r="E54" s="4">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55">
-        <v>0.1</v>
-      </c>
-      <c r="D55" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56">
-        <v>0.1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57">
-        <v>0.1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58">
-        <v>0.05</v>
-      </c>
-      <c r="D58" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59">
-        <v>0.1</v>
-      </c>
-      <c r="D59" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60">
-        <v>0.05</v>
-      </c>
-      <c r="D60" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61">
-        <v>0.1</v>
-      </c>
-      <c r="D61" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>